<commit_message>
agregue el sistema de plantillas
</commit_message>
<xml_diff>
--- a/datos_guardados.xlsx
+++ b/datos_guardados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>id_user</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>2024-05-15</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>hueheu</t>
+  </si>
+  <si>
+    <t>2023-05-11</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>dsfa</t>
   </si>
 </sst>
 </file>
@@ -326,7 +341,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -392,6 +407,26 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>